<commit_message>
corrected columns in scribe notes
</commit_message>
<xml_diff>
--- a/2024AgileCupMetadata_ScribeNotes_CameraInfo.xlsx
+++ b/2024AgileCupMetadata_ScribeNotes_CameraInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashob\Dropbox\ADHN\AgileCup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charles/Documents/Software Dev/twentyfour_agile_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="177" documentId="13_ncr:1_{A5030E19-6A4E-4CA3-8F9A-A7704359E8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07F4BA6F-E019-4DF1-BDBE-9C61E94E2FE4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026312AE-6881-D247-BECA-131C13461143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="1440" windowWidth="23490" windowHeight="13800" firstSheet="2" xr2:uid="{AEF2495E-096E-4216-9B6D-1CD8BB76D740}"/>
+    <workbookView xWindow="2720" yWindow="1440" windowWidth="23500" windowHeight="13800" xr2:uid="{AEF2495E-096E-4216-9B6D-1CD8BB76D740}"/>
   </bookViews>
   <sheets>
     <sheet name="MStd" sheetId="9" r:id="rId1"/>
@@ -1705,7 +1705,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1717,19 +1717,18 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Helvetica"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2132,25 +2131,25 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="I2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="9" max="9" width="61" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
-    <col min="15" max="15" width="22.42578125" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" customWidth="1"/>
+    <col min="11" max="11" width="22.5" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="26.83203125" customWidth="1"/>
+    <col min="14" max="14" width="20.1640625" customWidth="1"/>
+    <col min="15" max="15" width="22.5" customWidth="1"/>
+    <col min="16" max="16" width="20.1640625" customWidth="1"/>
+    <col min="17" max="17" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2203,15 +2202,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
       </c>
       <c r="D2">
         <v>45.15</v>
@@ -2232,15 +2231,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
       </c>
       <c r="D3">
         <v>42.83</v>
@@ -2276,15 +2275,15 @@
         <v>0.39358796296296295</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>24</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
       </c>
       <c r="D4">
         <v>54.65</v>
@@ -2320,15 +2319,15 @@
         <v>0.39537037037037037</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>24</v>
       </c>
       <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
       </c>
       <c r="D5">
         <v>58.95</v>
@@ -2364,15 +2363,15 @@
         <v>0.39719907407407407</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>24</v>
       </c>
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
       </c>
       <c r="D6">
         <v>45.34</v>
@@ -2408,15 +2407,15 @@
         <v>0.39856481481481482</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>24</v>
       </c>
       <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
         <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
       </c>
       <c r="D7">
         <v>50.5</v>
@@ -2458,15 +2457,15 @@
         <v>0.40122685185185186</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>24</v>
       </c>
       <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
         <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
       </c>
       <c r="D8">
         <v>42.17</v>
@@ -2502,15 +2501,15 @@
         <v>0.40327546296296296</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>24</v>
       </c>
       <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>52</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
       </c>
       <c r="D9">
         <v>60.3</v>
@@ -2549,15 +2548,15 @@
         <v>0.40474537037037039</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16</v>
       </c>
       <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
         <v>56</v>
-      </c>
-      <c r="C10" t="s">
-        <v>57</v>
       </c>
       <c r="D10">
         <v>57.68</v>
@@ -2590,15 +2589,15 @@
         <v>0.40802083333333333</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
         <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>62</v>
       </c>
       <c r="D11">
         <v>38.44</v>
@@ -2631,15 +2630,15 @@
         <v>0.40912037037037036</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>16</v>
       </c>
       <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
         <v>66</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
       </c>
       <c r="D12">
         <v>44.88</v>
@@ -2675,15 +2674,15 @@
         <v>0.41035879629629629</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>16</v>
       </c>
       <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
         <v>71</v>
-      </c>
-      <c r="C13" t="s">
-        <v>72</v>
       </c>
       <c r="D13">
         <v>33.15</v>
@@ -2722,15 +2721,15 @@
         <v>0.41166666666666668</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>16</v>
       </c>
       <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
         <v>77</v>
-      </c>
-      <c r="C14" t="s">
-        <v>78</v>
       </c>
       <c r="D14">
         <v>38.659999999999997</v>
@@ -2769,15 +2768,15 @@
         <v>0.41312500000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>16</v>
       </c>
       <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
         <v>82</v>
-      </c>
-      <c r="C15" t="s">
-        <v>83</v>
       </c>
       <c r="D15">
         <v>49</v>
@@ -2810,15 +2809,15 @@
         <v>0.41460648148148149</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
         <v>87</v>
-      </c>
-      <c r="C16" t="s">
-        <v>88</v>
       </c>
       <c r="D16">
         <v>49.19</v>
@@ -2854,15 +2853,15 @@
         <v>0.41646990740740741</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
         <v>92</v>
-      </c>
-      <c r="C17" t="s">
-        <v>93</v>
       </c>
       <c r="D17">
         <v>75</v>
@@ -2898,15 +2897,15 @@
         <v>0.41846064814814815</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" t="s">
         <v>97</v>
-      </c>
-      <c r="C18" t="s">
-        <v>98</v>
       </c>
       <c r="D18">
         <v>40.340000000000003</v>
@@ -2945,15 +2944,15 @@
         <v>0.41956018518518517</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" t="s">
         <v>102</v>
-      </c>
-      <c r="C19" t="s">
-        <v>103</v>
       </c>
       <c r="D19">
         <v>75</v>
@@ -2989,15 +2988,15 @@
         <v>0.42129629629629628</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" t="s">
         <v>107</v>
-      </c>
-      <c r="C20" t="s">
-        <v>108</v>
       </c>
       <c r="D20">
         <v>59.8</v>
@@ -3033,15 +3032,15 @@
         <v>0.42290509259259257</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>16</v>
       </c>
       <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
         <v>112</v>
-      </c>
-      <c r="C21" t="s">
-        <v>57</v>
       </c>
       <c r="D21">
         <v>41.05</v>
@@ -3074,15 +3073,15 @@
         <v>0.42405092592592591</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8</v>
       </c>
       <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
         <v>116</v>
-      </c>
-      <c r="C22" t="s">
-        <v>117</v>
       </c>
       <c r="D22">
         <v>56.49</v>
@@ -3118,15 +3117,15 @@
         <v>0.42725694444444445</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
       <c r="B23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" t="s">
         <v>121</v>
-      </c>
-      <c r="C23" t="s">
-        <v>122</v>
       </c>
       <c r="D23">
         <v>40.43</v>
@@ -3159,15 +3158,15 @@
         <v>0.4287037037037037</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>8</v>
       </c>
       <c r="B24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" t="s">
         <v>126</v>
-      </c>
-      <c r="C24" t="s">
-        <v>127</v>
       </c>
       <c r="D24">
         <v>43.19</v>
@@ -3203,15 +3202,15 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
       <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
         <v>132</v>
-      </c>
-      <c r="C25" t="s">
-        <v>62</v>
       </c>
       <c r="D25">
         <v>42.12</v>
@@ -3247,15 +3246,15 @@
         <v>0.43106481481481479</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
       <c r="B26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" t="s">
         <v>136</v>
-      </c>
-      <c r="C26" t="s">
-        <v>137</v>
       </c>
       <c r="D26">
         <v>75</v>
@@ -3291,15 +3290,15 @@
         <v>0.43320601851851853</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>8</v>
       </c>
       <c r="B27" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" t="s">
         <v>141</v>
-      </c>
-      <c r="C27" t="s">
-        <v>142</v>
       </c>
       <c r="D27">
         <v>51.11</v>
@@ -3332,15 +3331,15 @@
         <v>0.43471064814814814</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>8</v>
       </c>
       <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
         <v>146</v>
-      </c>
-      <c r="C28" t="s">
-        <v>67</v>
       </c>
       <c r="D28">
         <v>48.43</v>
@@ -3373,15 +3372,15 @@
         <v>0.43599537037037039</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>8</v>
       </c>
       <c r="B29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" t="s">
         <v>150</v>
-      </c>
-      <c r="C29" t="s">
-        <v>151</v>
       </c>
       <c r="D29">
         <v>48.73</v>
@@ -3414,15 +3413,15 @@
         <v>0.43722222222222223</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>8</v>
       </c>
       <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" t="s">
         <v>155</v>
-      </c>
-      <c r="C30" t="s">
-        <v>117</v>
       </c>
       <c r="D30">
         <v>52.19</v>
@@ -3458,15 +3457,15 @@
         <v>0.43874999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>12</v>
       </c>
       <c r="B31" t="s">
+        <v>161</v>
+      </c>
+      <c r="C31" t="s">
         <v>160</v>
-      </c>
-      <c r="C31" t="s">
-        <v>161</v>
       </c>
       <c r="D31">
         <v>59.79</v>
@@ -3508,15 +3507,15 @@
         <v>0.44268518518518518</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>12</v>
       </c>
       <c r="B32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" t="s">
         <v>166</v>
-      </c>
-      <c r="C32" t="s">
-        <v>167</v>
       </c>
       <c r="D32">
         <v>31.37</v>
@@ -3552,15 +3551,15 @@
         <v>0.44408564814814816</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>12</v>
       </c>
       <c r="B33" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" t="s">
         <v>171</v>
-      </c>
-      <c r="C33" t="s">
-        <v>172</v>
       </c>
       <c r="D33">
         <v>39.700000000000003</v>
@@ -3599,15 +3598,15 @@
         <v>0.44570601851851854</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>20</v>
       </c>
       <c r="B34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" t="s">
         <v>177</v>
-      </c>
-      <c r="C34" t="s">
-        <v>98</v>
       </c>
       <c r="D34">
         <v>57.01</v>
@@ -3643,15 +3642,15 @@
         <v>0.44828703703703704</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>20</v>
       </c>
       <c r="B35" t="s">
+        <v>182</v>
+      </c>
+      <c r="C35" t="s">
         <v>181</v>
-      </c>
-      <c r="C35" t="s">
-        <v>182</v>
       </c>
       <c r="D35">
         <v>46.34</v>
@@ -3690,15 +3689,15 @@
         <v>0.45068287037037036</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20</v>
       </c>
       <c r="B36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
         <v>186</v>
-      </c>
-      <c r="C36" t="s">
-        <v>72</v>
       </c>
       <c r="D36">
         <v>35.590000000000003</v>
@@ -3731,15 +3730,15 @@
         <v>0.45185185185185184</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>20</v>
       </c>
       <c r="B37" t="s">
+        <v>191</v>
+      </c>
+      <c r="C37" t="s">
         <v>190</v>
-      </c>
-      <c r="C37" t="s">
-        <v>191</v>
       </c>
       <c r="D37">
         <v>47.97</v>
@@ -3778,15 +3777,15 @@
         <v>0.4533564814814815</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>20</v>
       </c>
       <c r="B38" t="s">
+        <v>197</v>
+      </c>
+      <c r="C38" t="s">
         <v>196</v>
-      </c>
-      <c r="C38" t="s">
-        <v>197</v>
       </c>
       <c r="D38">
         <v>40.700000000000003</v>
@@ -3828,15 +3827,15 @@
         <v>0.45505787037037038</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>20</v>
       </c>
       <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s">
         <v>201</v>
-      </c>
-      <c r="C39" t="s">
-        <v>78</v>
       </c>
       <c r="D39">
         <v>46.36</v>
@@ -3872,15 +3871,15 @@
         <v>0.45656249999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>20</v>
       </c>
       <c r="B40" t="s">
+        <v>206</v>
+      </c>
+      <c r="C40" t="s">
         <v>205</v>
-      </c>
-      <c r="C40" t="s">
-        <v>206</v>
       </c>
       <c r="D40">
         <v>49.33</v>
@@ -3919,15 +3918,15 @@
         <v>0.45793981481481483</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>20</v>
       </c>
       <c r="B41" t="s">
+        <v>211</v>
+      </c>
+      <c r="C41" t="s">
         <v>210</v>
-      </c>
-      <c r="C41" t="s">
-        <v>211</v>
       </c>
       <c r="D41">
         <v>50.31</v>
@@ -3960,15 +3959,15 @@
         <v>0.45943287037037039</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>20</v>
       </c>
       <c r="B42" t="s">
+        <v>216</v>
+      </c>
+      <c r="C42" t="s">
         <v>215</v>
-      </c>
-      <c r="C42" t="s">
-        <v>216</v>
       </c>
       <c r="D42">
         <v>75</v>
@@ -4007,15 +4006,15 @@
         <v>0.46133101851851854</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>20</v>
       </c>
       <c r="B43" t="s">
+        <v>222</v>
+      </c>
+      <c r="C43" t="s">
         <v>221</v>
-      </c>
-      <c r="C43" t="s">
-        <v>222</v>
       </c>
       <c r="D43">
         <v>34.6</v>
@@ -4048,15 +4047,15 @@
         <v>0.4629050925925926</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>20</v>
       </c>
       <c r="B44" t="s">
+        <v>227</v>
+      </c>
+      <c r="C44" t="s">
         <v>226</v>
-      </c>
-      <c r="C44" t="s">
-        <v>227</v>
       </c>
       <c r="D44">
         <v>36.19</v>
@@ -4092,15 +4091,15 @@
         <v>0.46457175925925925</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>20</v>
       </c>
       <c r="B45" t="s">
+        <v>232</v>
+      </c>
+      <c r="C45" t="s">
         <v>231</v>
-      </c>
-      <c r="C45" t="s">
-        <v>232</v>
       </c>
       <c r="D45">
         <v>45.44</v>
@@ -4136,15 +4135,15 @@
         <v>0.4659490740740741</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>20</v>
       </c>
       <c r="B46" t="s">
+        <v>237</v>
+      </c>
+      <c r="C46" t="s">
         <v>236</v>
-      </c>
-      <c r="C46" t="s">
-        <v>237</v>
       </c>
       <c r="D46">
         <v>60.06</v>
@@ -4183,15 +4182,15 @@
         <v>0.46748842592592593</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>20</v>
       </c>
       <c r="B47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" t="s">
         <v>241</v>
-      </c>
-      <c r="C47" t="s">
-        <v>98</v>
       </c>
       <c r="D47">
         <v>42.06</v>
@@ -4231,9 +4230,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
-    <sortCondition ref="C2:C12"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -4244,23 +4240,23 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="J2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O7" sqref="O7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="9" max="9" width="55.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="11" max="12" width="22.42578125" customWidth="1"/>
-    <col min="13" max="14" width="20.140625" customWidth="1"/>
-    <col min="15" max="15" width="22.42578125" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="9" max="9" width="55.6640625" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" customWidth="1"/>
+    <col min="11" max="12" width="22.5" customWidth="1"/>
+    <col min="13" max="14" width="20.1640625" customWidth="1"/>
+    <col min="15" max="15" width="22.5" customWidth="1"/>
+    <col min="16" max="16" width="20.1640625" customWidth="1"/>
+    <col min="17" max="17" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4313,15 +4309,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
       </c>
       <c r="D2">
         <v>44.4</v>
@@ -4354,15 +4350,15 @@
         <v>0.49769675925925927</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
       </c>
       <c r="D3">
         <v>45.29</v>
@@ -4398,15 +4394,15 @@
         <v>0.50108796296296299</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>24</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
       </c>
       <c r="D4">
         <v>71.540000000000006</v>
@@ -4445,15 +4441,15 @@
         <v>0.50300925925925921</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>24</v>
       </c>
       <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
       </c>
       <c r="D5">
         <v>68.400000000000006</v>
@@ -4489,15 +4485,15 @@
         <v>0.50471064814814814</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>24</v>
       </c>
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
       </c>
       <c r="D6">
         <v>48.5</v>
@@ -4533,15 +4529,15 @@
         <v>0.50614583333333329</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>24</v>
       </c>
       <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
         <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
       </c>
       <c r="D7">
         <v>51.5</v>
@@ -4571,15 +4567,15 @@
         <v>0.50789351851851849</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>24</v>
       </c>
       <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
         <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
       </c>
       <c r="D8">
         <v>49.54</v>
@@ -4609,15 +4605,15 @@
         <v>0.50958333333333339</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>24</v>
       </c>
       <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>52</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
       </c>
       <c r="D9">
         <v>47.84</v>
@@ -4650,15 +4646,15 @@
         <v>0.51111111111111107</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16</v>
       </c>
       <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
         <v>56</v>
-      </c>
-      <c r="C10" t="s">
-        <v>57</v>
       </c>
       <c r="D10">
         <v>67.23</v>
@@ -4694,15 +4690,15 @@
         <v>0.51409722222222221</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
         <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>62</v>
       </c>
       <c r="D11">
         <v>49.49</v>
@@ -4738,15 +4734,15 @@
         <v>0.51565972222222223</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>16</v>
       </c>
       <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
         <v>66</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
       </c>
       <c r="D12">
         <v>62.19</v>
@@ -4782,15 +4778,15 @@
         <v>0.51728009259259256</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>16</v>
       </c>
       <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
         <v>71</v>
-      </c>
-      <c r="C13" t="s">
-        <v>72</v>
       </c>
       <c r="D13">
         <v>55.04</v>
@@ -4826,15 +4822,15 @@
         <v>0.51866898148148144</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>16</v>
       </c>
       <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
         <v>77</v>
-      </c>
-      <c r="C14" t="s">
-        <v>78</v>
       </c>
       <c r="D14">
         <v>54.14</v>
@@ -4873,15 +4869,15 @@
         <v>0.52021990740740742</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>16</v>
       </c>
       <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
         <v>82</v>
-      </c>
-      <c r="C15" t="s">
-        <v>83</v>
       </c>
       <c r="D15">
         <v>65.16</v>
@@ -4920,15 +4916,15 @@
         <v>0.52174768518518522</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
         <v>87</v>
-      </c>
-      <c r="C16" t="s">
-        <v>88</v>
       </c>
       <c r="D16">
         <v>53.72</v>
@@ -4961,15 +4957,15 @@
         <v>0.52337962962962958</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
         <v>92</v>
-      </c>
-      <c r="C17" t="s">
-        <v>93</v>
       </c>
       <c r="D17">
         <v>62.92</v>
@@ -5008,15 +5004,15 @@
         <v>0.52489583333333334</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" t="s">
         <v>97</v>
-      </c>
-      <c r="C18" t="s">
-        <v>98</v>
       </c>
       <c r="D18">
         <v>46.05</v>
@@ -5055,15 +5051,15 @@
         <v>0.52619212962962958</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" t="s">
         <v>102</v>
-      </c>
-      <c r="C19" t="s">
-        <v>103</v>
       </c>
       <c r="D19">
         <v>75</v>
@@ -5099,15 +5095,15 @@
         <v>0.52798611111111116</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" t="s">
         <v>107</v>
-      </c>
-      <c r="C20" t="s">
-        <v>108</v>
       </c>
       <c r="D20">
         <v>75</v>
@@ -5143,15 +5139,15 @@
         <v>0.52953703703703703</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>16</v>
       </c>
       <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
         <v>112</v>
-      </c>
-      <c r="C21" t="s">
-        <v>57</v>
       </c>
       <c r="D21">
         <v>56.68</v>
@@ -5190,15 +5186,15 @@
         <v>0.53104166666666663</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8</v>
       </c>
       <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
         <v>116</v>
-      </c>
-      <c r="C22" t="s">
-        <v>117</v>
       </c>
       <c r="D22">
         <v>54.37</v>
@@ -5231,15 +5227,15 @@
         <v>0.53418981481481487</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
       <c r="B23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" t="s">
         <v>121</v>
-      </c>
-      <c r="C23" t="s">
-        <v>122</v>
       </c>
       <c r="D23">
         <v>45.8</v>
@@ -5272,15 +5268,15 @@
         <v>0.53559027777777779</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>8</v>
       </c>
       <c r="B24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" t="s">
         <v>126</v>
-      </c>
-      <c r="C24" t="s">
-        <v>127</v>
       </c>
       <c r="D24">
         <v>49.03</v>
@@ -5313,15 +5309,15 @@
         <v>0.53697916666666667</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
       <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
         <v>132</v>
-      </c>
-      <c r="C25" t="s">
-        <v>62</v>
       </c>
       <c r="D25">
         <v>38.39</v>
@@ -5354,15 +5350,15 @@
         <v>0.53822916666666665</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
       <c r="B26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" t="s">
         <v>136</v>
-      </c>
-      <c r="C26" t="s">
-        <v>137</v>
       </c>
       <c r="D26">
         <v>75</v>
@@ -5401,15 +5397,15 @@
         <v>0.53997685185185185</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>8</v>
       </c>
       <c r="B27" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" t="s">
         <v>141</v>
-      </c>
-      <c r="C27" t="s">
-        <v>142</v>
       </c>
       <c r="D27">
         <v>69.92</v>
@@ -5445,15 +5441,15 @@
         <v>0.54592592592592593</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>8</v>
       </c>
       <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
         <v>146</v>
-      </c>
-      <c r="C28" t="s">
-        <v>67</v>
       </c>
       <c r="D28">
         <v>58.87</v>
@@ -5486,15 +5482,15 @@
         <v>0.54752314814814818</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>8</v>
       </c>
       <c r="B29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" t="s">
         <v>150</v>
-      </c>
-      <c r="C29" t="s">
-        <v>151</v>
       </c>
       <c r="D29">
         <v>55.04</v>
@@ -5533,15 +5529,15 @@
         <v>0.54890046296296291</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>8</v>
       </c>
       <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" t="s">
         <v>155</v>
-      </c>
-      <c r="C30" t="s">
-        <v>117</v>
       </c>
       <c r="D30">
         <v>75</v>
@@ -5580,15 +5576,15 @@
         <v>0.55083333333333329</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>12</v>
       </c>
       <c r="B31" t="s">
+        <v>161</v>
+      </c>
+      <c r="C31" t="s">
         <v>160</v>
-      </c>
-      <c r="C31" t="s">
-        <v>161</v>
       </c>
       <c r="D31">
         <v>63.35</v>
@@ -5627,15 +5623,15 @@
         <v>0.55341435185185184</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>12</v>
       </c>
       <c r="B32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" t="s">
         <v>166</v>
-      </c>
-      <c r="C32" t="s">
-        <v>167</v>
       </c>
       <c r="D32">
         <v>35.119999999999997</v>
@@ -5668,15 +5664,15 @@
         <v>0.55462962962962958</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>12</v>
       </c>
       <c r="B33" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" t="s">
         <v>171</v>
-      </c>
-      <c r="C33" t="s">
-        <v>172</v>
       </c>
       <c r="D33">
         <v>40.76</v>
@@ -5712,15 +5708,15 @@
         <v>0.55635416666666671</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>20</v>
       </c>
       <c r="B34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" t="s">
         <v>177</v>
-      </c>
-      <c r="C34" t="s">
-        <v>98</v>
       </c>
       <c r="D34">
         <v>75</v>
@@ -5756,15 +5752,15 @@
         <v>0.55899305555555556</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>20</v>
       </c>
       <c r="B35" t="s">
+        <v>182</v>
+      </c>
+      <c r="C35" t="s">
         <v>181</v>
-      </c>
-      <c r="C35" t="s">
-        <v>182</v>
       </c>
       <c r="D35">
         <v>75</v>
@@ -5803,15 +5799,15 @@
         <v>0.56087962962962967</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20</v>
       </c>
       <c r="B36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
         <v>186</v>
-      </c>
-      <c r="C36" t="s">
-        <v>72</v>
       </c>
       <c r="D36">
         <v>44.62</v>
@@ -5847,15 +5843,15 @@
         <v>0.56259259259259264</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>20</v>
       </c>
       <c r="B37" t="s">
+        <v>191</v>
+      </c>
+      <c r="C37" t="s">
         <v>190</v>
-      </c>
-      <c r="C37" t="s">
-        <v>191</v>
       </c>
       <c r="D37">
         <v>55.81</v>
@@ -5894,15 +5890,15 @@
         <v>0.56414351851851852</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>20</v>
       </c>
       <c r="B38" t="s">
+        <v>197</v>
+      </c>
+      <c r="C38" t="s">
         <v>196</v>
-      </c>
-      <c r="C38" t="s">
-        <v>197</v>
       </c>
       <c r="D38">
         <v>40.270000000000003</v>
@@ -5935,15 +5931,15 @@
         <v>0.56543981481481487</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>20</v>
       </c>
       <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s">
         <v>201</v>
-      </c>
-      <c r="C39" t="s">
-        <v>78</v>
       </c>
       <c r="D39">
         <v>51.06</v>
@@ -5982,15 +5978,15 @@
         <v>0.5668171296296296</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>20</v>
       </c>
       <c r="B40" t="s">
+        <v>206</v>
+      </c>
+      <c r="C40" t="s">
         <v>205</v>
-      </c>
-      <c r="C40" t="s">
-        <v>206</v>
       </c>
       <c r="D40">
         <v>37.25</v>
@@ -6017,15 +6013,15 @@
         <v>0.56822916666666667</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>20</v>
       </c>
       <c r="B41" t="s">
+        <v>211</v>
+      </c>
+      <c r="C41" t="s">
         <v>210</v>
-      </c>
-      <c r="C41" t="s">
-        <v>211</v>
       </c>
       <c r="D41">
         <v>60.91</v>
@@ -6055,15 +6051,15 @@
         <v>0.56972222222222224</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>20</v>
       </c>
       <c r="B42" t="s">
+        <v>216</v>
+      </c>
+      <c r="C42" t="s">
         <v>215</v>
-      </c>
-      <c r="C42" t="s">
-        <v>216</v>
       </c>
       <c r="D42">
         <v>75</v>
@@ -6093,15 +6089,15 @@
         <v>0.5713773148148148</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>20</v>
       </c>
       <c r="B43" t="s">
+        <v>222</v>
+      </c>
+      <c r="C43" t="s">
         <v>221</v>
-      </c>
-      <c r="C43" t="s">
-        <v>222</v>
       </c>
       <c r="D43">
         <v>35.619999999999997</v>
@@ -6131,15 +6127,15 @@
         <v>0.57256944444444446</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>20</v>
       </c>
       <c r="B44" t="s">
+        <v>227</v>
+      </c>
+      <c r="C44" t="s">
         <v>226</v>
-      </c>
-      <c r="C44" t="s">
-        <v>227</v>
       </c>
       <c r="D44">
         <v>39.08</v>
@@ -6169,15 +6165,15 @@
         <v>0.57393518518518516</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>20</v>
       </c>
       <c r="B45" t="s">
+        <v>232</v>
+      </c>
+      <c r="C45" t="s">
         <v>231</v>
-      </c>
-      <c r="C45" t="s">
-        <v>232</v>
       </c>
       <c r="D45">
         <v>40.56</v>
@@ -6207,15 +6203,15 @@
         <v>0.57524305555555555</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>20</v>
       </c>
       <c r="B46" t="s">
+        <v>237</v>
+      </c>
+      <c r="C46" t="s">
         <v>236</v>
-      </c>
-      <c r="C46" t="s">
-        <v>237</v>
       </c>
       <c r="D46">
         <v>54.06</v>
@@ -6248,15 +6244,15 @@
         <v>0.57670138888888889</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>20</v>
       </c>
       <c r="B47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" t="s">
         <v>241</v>
-      </c>
-      <c r="C47" t="s">
-        <v>98</v>
       </c>
       <c r="D47" t="s">
         <v>347</v>
@@ -6301,31 +6297,31 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P34" sqref="P34"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
     <col min="9" max="9" width="51" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="11" max="12" width="22.42578125" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
-    <col min="15" max="15" width="22.42578125" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" customWidth="1"/>
+    <col min="11" max="12" width="22.5" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" customWidth="1"/>
+    <col min="14" max="14" width="20.1640625" customWidth="1"/>
+    <col min="15" max="15" width="22.5" customWidth="1"/>
+    <col min="16" max="16" width="20.1640625" customWidth="1"/>
+    <col min="17" max="17" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -6370,15 +6366,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
       </c>
       <c r="D2">
         <v>43.37</v>
@@ -6414,15 +6410,15 @@
         <v>0.60371527777777778</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
       </c>
       <c r="D3">
         <v>35.51</v>
@@ -6455,15 +6451,15 @@
         <v>0.60483796296296299</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>24</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
       </c>
       <c r="D4">
         <v>60</v>
@@ -6499,15 +6495,15 @@
         <v>0.60640046296296302</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>24</v>
       </c>
       <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
       </c>
       <c r="D5">
         <v>60</v>
@@ -6543,15 +6539,15 @@
         <v>0.60781249999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>24</v>
       </c>
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
       </c>
       <c r="D6">
         <v>39.409999999999997</v>
@@ -6587,15 +6583,15 @@
         <v>0.608912037037037</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>24</v>
       </c>
       <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
         <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
       </c>
       <c r="D7">
         <v>60</v>
@@ -6634,15 +6630,15 @@
         <v>0.61037037037037034</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>24</v>
       </c>
       <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
         <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
       </c>
       <c r="D8">
         <v>49.74</v>
@@ -6681,15 +6677,15 @@
         <v>0.61171296296296296</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>24</v>
       </c>
       <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>52</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
       </c>
       <c r="D9">
         <v>50.03</v>
@@ -6728,15 +6724,15 @@
         <v>0.61293981481481485</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16</v>
       </c>
       <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
         <v>56</v>
-      </c>
-      <c r="C10" t="s">
-        <v>57</v>
       </c>
       <c r="D10">
         <v>40.46</v>
@@ -6769,15 +6765,15 @@
         <v>0.61509259259259264</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>237</v>
+      </c>
+      <c r="C11" t="s">
         <v>370</v>
-      </c>
-      <c r="C11" t="s">
-        <v>237</v>
       </c>
       <c r="D11">
         <v>46.63</v>
@@ -6813,15 +6809,15 @@
         <v>0.61637731481481484</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>16</v>
       </c>
       <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
         <v>61</v>
-      </c>
-      <c r="C12" t="s">
-        <v>62</v>
       </c>
       <c r="D12">
         <v>37.31</v>
@@ -6854,15 +6850,15 @@
         <v>0.61754629629629632</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>16</v>
       </c>
       <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
         <v>66</v>
-      </c>
-      <c r="C13" t="s">
-        <v>67</v>
       </c>
       <c r="D13">
         <v>51.27</v>
@@ -6895,15 +6891,15 @@
         <v>0.61870370370370376</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>16</v>
       </c>
       <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
         <v>71</v>
-      </c>
-      <c r="C14" t="s">
-        <v>72</v>
       </c>
       <c r="D14">
         <v>34.15</v>
@@ -6942,15 +6938,15 @@
         <v>0.61971064814814814</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>16</v>
       </c>
       <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
         <v>77</v>
-      </c>
-      <c r="C15" t="s">
-        <v>78</v>
       </c>
       <c r="D15">
         <v>37.200000000000003</v>
@@ -6986,15 +6982,15 @@
         <v>0.62081018518518516</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
         <v>82</v>
-      </c>
-      <c r="C16" t="s">
-        <v>83</v>
       </c>
       <c r="D16">
         <v>51.73</v>
@@ -7027,15 +7023,15 @@
         <v>0.62203703703703705</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
         <v>87</v>
-      </c>
-      <c r="C17" t="s">
-        <v>88</v>
       </c>
       <c r="D17">
         <v>60</v>
@@ -7071,15 +7067,15 @@
         <v>0.62333333333333329</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" t="s">
         <v>92</v>
-      </c>
-      <c r="C18" t="s">
-        <v>93</v>
       </c>
       <c r="D18">
         <v>60</v>
@@ -7115,15 +7111,15 @@
         <v>0.62479166666666663</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
         <v>97</v>
-      </c>
-      <c r="C19" t="s">
-        <v>98</v>
       </c>
       <c r="D19">
         <v>36.67</v>
@@ -7159,15 +7155,15 @@
         <v>0.62574074074074071</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
         <v>112</v>
-      </c>
-      <c r="C20" t="s">
-        <v>57</v>
       </c>
       <c r="D20">
         <v>41.28</v>
@@ -7206,15 +7202,15 @@
         <v>0.62703703703703706</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8</v>
       </c>
       <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" t="s">
         <v>116</v>
-      </c>
-      <c r="C21" t="s">
-        <v>117</v>
       </c>
       <c r="D21">
         <v>44.23</v>
@@ -7250,15 +7246,15 @@
         <v>0.62981481481481483</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8</v>
       </c>
       <c r="B22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" t="s">
         <v>121</v>
-      </c>
-      <c r="C22" t="s">
-        <v>122</v>
       </c>
       <c r="D22">
         <v>47.11</v>
@@ -7291,15 +7287,15 @@
         <v>0.63114583333333329</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
       <c r="B23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" t="s">
         <v>126</v>
-      </c>
-      <c r="C23" t="s">
-        <v>127</v>
       </c>
       <c r="D23">
         <v>39.479999999999997</v>
@@ -7332,15 +7328,15 @@
         <v>0.63237268518518519</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>8</v>
       </c>
       <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
         <v>132</v>
-      </c>
-      <c r="C24" t="s">
-        <v>62</v>
       </c>
       <c r="D24">
         <v>35.33</v>
@@ -7376,15 +7372,15 @@
         <v>0.63339120370370372</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
       <c r="B25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" t="s">
         <v>136</v>
-      </c>
-      <c r="C25" t="s">
-        <v>137</v>
       </c>
       <c r="D25">
         <v>60</v>
@@ -7420,15 +7416,15 @@
         <v>0.63489583333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
       <c r="B26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" t="s">
         <v>141</v>
-      </c>
-      <c r="C26" t="s">
-        <v>142</v>
       </c>
       <c r="D26">
         <v>58.22</v>
@@ -7464,15 +7460,15 @@
         <v>0.63604166666666662</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>8</v>
       </c>
       <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" t="s">
         <v>146</v>
-      </c>
-      <c r="C27" t="s">
-        <v>67</v>
       </c>
       <c r="D27">
         <v>57.15</v>
@@ -7505,15 +7501,15 @@
         <v>0.63732638888888893</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>8</v>
       </c>
       <c r="B28" t="s">
+        <v>151</v>
+      </c>
+      <c r="C28" t="s">
         <v>150</v>
-      </c>
-      <c r="C28" t="s">
-        <v>151</v>
       </c>
       <c r="D28">
         <v>45.08</v>
@@ -7546,15 +7542,15 @@
         <v>0.63847222222222222</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>8</v>
       </c>
       <c r="B29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" t="s">
         <v>155</v>
-      </c>
-      <c r="C29" t="s">
-        <v>117</v>
       </c>
       <c r="D29">
         <v>54.45</v>
@@ -7587,15 +7583,15 @@
         <v>0.63976851851851857</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
       <c r="B30" t="s">
+        <v>161</v>
+      </c>
+      <c r="C30" t="s">
         <v>160</v>
-      </c>
-      <c r="C30" t="s">
-        <v>161</v>
       </c>
       <c r="D30">
         <v>47.85</v>
@@ -7634,15 +7630,15 @@
         <v>0.64247685185185188</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>12</v>
       </c>
       <c r="B31" t="s">
+        <v>167</v>
+      </c>
+      <c r="C31" t="s">
         <v>166</v>
-      </c>
-      <c r="C31" t="s">
-        <v>167</v>
       </c>
       <c r="D31">
         <v>28.32</v>
@@ -7675,15 +7671,15 @@
         <v>0.64359953703703698</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>12</v>
       </c>
       <c r="B32" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" t="s">
         <v>171</v>
-      </c>
-      <c r="C32" t="s">
-        <v>172</v>
       </c>
       <c r="D32">
         <v>42.02</v>
@@ -7719,15 +7715,15 @@
         <v>0.64484953703703707</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>20</v>
       </c>
       <c r="B33" t="s">
+        <v>237</v>
+      </c>
+      <c r="C33" t="s">
         <v>416</v>
-      </c>
-      <c r="C33" t="s">
-        <v>237</v>
       </c>
       <c r="D33">
         <v>47.26</v>
@@ -7763,15 +7759,15 @@
         <v>0.64723379629629629</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>20</v>
       </c>
       <c r="B34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" t="s">
         <v>177</v>
-      </c>
-      <c r="C34" t="s">
-        <v>98</v>
       </c>
       <c r="D34">
         <v>36.450000000000003</v>
@@ -7806,15 +7802,15 @@
       <c r="P34" s="4"/>
       <c r="Q34" s="5"/>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>20</v>
       </c>
       <c r="B35" t="s">
+        <v>182</v>
+      </c>
+      <c r="C35" t="s">
         <v>181</v>
-      </c>
-      <c r="C35" t="s">
-        <v>182</v>
       </c>
       <c r="D35">
         <v>38.590000000000003</v>
@@ -7852,15 +7848,15 @@
       <c r="P35" s="4"/>
       <c r="Q35" s="5"/>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20</v>
       </c>
       <c r="B36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
         <v>186</v>
-      </c>
-      <c r="C36" t="s">
-        <v>72</v>
       </c>
       <c r="D36">
         <v>38.29</v>
@@ -7898,15 +7894,15 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="5"/>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>20</v>
       </c>
       <c r="B37" t="s">
+        <v>191</v>
+      </c>
+      <c r="C37" t="s">
         <v>190</v>
-      </c>
-      <c r="C37" t="s">
-        <v>191</v>
       </c>
       <c r="D37">
         <v>38.33</v>
@@ -7943,15 +7939,15 @@
       </c>
       <c r="P37" s="4"/>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>20</v>
       </c>
       <c r="B38" t="s">
+        <v>197</v>
+      </c>
+      <c r="C38" t="s">
         <v>196</v>
-      </c>
-      <c r="C38" t="s">
-        <v>197</v>
       </c>
       <c r="D38">
         <v>31.69</v>
@@ -7979,15 +7975,15 @@
       </c>
       <c r="P38" s="4"/>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>20</v>
       </c>
       <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s">
         <v>201</v>
-      </c>
-      <c r="C39" t="s">
-        <v>78</v>
       </c>
       <c r="D39">
         <v>46.45</v>
@@ -8021,15 +8017,15 @@
       </c>
       <c r="P39" s="4"/>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>20</v>
       </c>
       <c r="B40" t="s">
+        <v>206</v>
+      </c>
+      <c r="C40" t="s">
         <v>205</v>
-      </c>
-      <c r="C40" t="s">
-        <v>206</v>
       </c>
       <c r="D40">
         <v>34.56</v>
@@ -8060,15 +8056,15 @@
       </c>
       <c r="P40" s="4"/>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>20</v>
       </c>
       <c r="B41" t="s">
+        <v>211</v>
+      </c>
+      <c r="C41" t="s">
         <v>210</v>
-      </c>
-      <c r="C41" t="s">
-        <v>211</v>
       </c>
       <c r="D41">
         <v>60</v>
@@ -8099,15 +8095,15 @@
       </c>
       <c r="P41" s="4"/>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>20</v>
       </c>
       <c r="B42" t="s">
+        <v>216</v>
+      </c>
+      <c r="C42" t="s">
         <v>215</v>
-      </c>
-      <c r="C42" t="s">
-        <v>216</v>
       </c>
       <c r="D42">
         <v>60</v>
@@ -8138,15 +8134,15 @@
       </c>
       <c r="P42" s="4"/>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>20</v>
       </c>
       <c r="B43" t="s">
+        <v>222</v>
+      </c>
+      <c r="C43" t="s">
         <v>221</v>
-      </c>
-      <c r="C43" t="s">
-        <v>222</v>
       </c>
       <c r="D43">
         <v>33.43</v>
@@ -8177,15 +8173,15 @@
       </c>
       <c r="P43" s="4"/>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>20</v>
       </c>
       <c r="B44" t="s">
+        <v>227</v>
+      </c>
+      <c r="C44" t="s">
         <v>226</v>
-      </c>
-      <c r="C44" t="s">
-        <v>227</v>
       </c>
       <c r="D44">
         <v>34.97</v>
@@ -8219,15 +8215,15 @@
       </c>
       <c r="P44" s="4"/>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>20</v>
       </c>
       <c r="B45" t="s">
+        <v>232</v>
+      </c>
+      <c r="C45" t="s">
         <v>231</v>
-      </c>
-      <c r="C45" t="s">
-        <v>232</v>
       </c>
       <c r="D45">
         <v>37.85</v>
@@ -8258,15 +8254,15 @@
       </c>
       <c r="P45" s="4"/>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>20</v>
       </c>
       <c r="B46" t="s">
+        <v>237</v>
+      </c>
+      <c r="C46" t="s">
         <v>236</v>
-      </c>
-      <c r="C46" t="s">
-        <v>237</v>
       </c>
       <c r="D46">
         <v>55.85</v>
@@ -8308,33 +8304,33 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="K2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N39" sqref="N39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" customWidth="1"/>
+    <col min="11" max="11" width="22.5" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
-    <col min="15" max="15" width="22.42578125" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" customWidth="1"/>
+    <col min="13" max="13" width="19.5" customWidth="1"/>
+    <col min="14" max="14" width="20.1640625" customWidth="1"/>
+    <col min="15" max="15" width="22.5" customWidth="1"/>
+    <col min="16" max="16" width="20.1640625" customWidth="1"/>
+    <col min="17" max="17" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -8379,15 +8375,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
       </c>
       <c r="D2">
         <v>47.75</v>
@@ -8423,15 +8419,15 @@
         <v>0.6943287037037037</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
       </c>
       <c r="D3">
         <v>54.15</v>
@@ -8470,15 +8466,15 @@
         <v>0.69472222222222224</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>24</v>
       </c>
       <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
       </c>
       <c r="D4">
         <v>60</v>
@@ -8514,15 +8510,15 @@
         <v>0.69670138888888888</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>24</v>
       </c>
       <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
         <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
       </c>
       <c r="D5">
         <v>60</v>
@@ -8561,15 +8557,15 @@
         <v>0.69870370370370372</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>24</v>
       </c>
       <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
         <v>47</v>
-      </c>
-      <c r="C6" t="s">
-        <v>48</v>
       </c>
       <c r="D6">
         <v>60</v>
@@ -8608,15 +8604,15 @@
         <v>0.70024305555555555</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>24</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
       </c>
       <c r="D7">
         <v>60</v>
@@ -8652,15 +8648,15 @@
         <v>0.70181712962962961</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>16</v>
       </c>
       <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
         <v>56</v>
-      </c>
-      <c r="C8" t="s">
-        <v>57</v>
       </c>
       <c r="D8">
         <v>49.69</v>
@@ -8699,15 +8695,15 @@
         <v>0.70427083333333329</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>16</v>
       </c>
       <c r="B9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" t="s">
         <v>370</v>
-      </c>
-      <c r="C9" t="s">
-        <v>237</v>
       </c>
       <c r="D9">
         <v>60</v>
@@ -8743,15 +8739,15 @@
         <v>0.70562499999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="25.5">
+    <row r="10" spans="1:17" ht="27" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16</v>
       </c>
       <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
         <v>61</v>
-      </c>
-      <c r="C10" t="s">
-        <v>62</v>
       </c>
       <c r="D10">
         <v>44.58</v>
@@ -8787,15 +8783,15 @@
         <v>483</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="25.5">
+    <row r="11" spans="1:17" ht="27" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
         <v>77</v>
-      </c>
-      <c r="C11" t="s">
-        <v>78</v>
       </c>
       <c r="D11">
         <v>55.8</v>
@@ -8834,15 +8830,15 @@
         <v>483</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="25.5">
+    <row r="12" spans="1:17" ht="27" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>16</v>
       </c>
       <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
         <v>82</v>
-      </c>
-      <c r="C12" t="s">
-        <v>83</v>
       </c>
       <c r="D12">
         <v>51.95</v>
@@ -8881,15 +8877,15 @@
         <v>483</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="25.5">
+    <row r="13" spans="1:17" ht="27" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>16</v>
       </c>
       <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
         <v>87</v>
-      </c>
-      <c r="C13" t="s">
-        <v>88</v>
       </c>
       <c r="D13">
         <v>60</v>
@@ -8925,15 +8921,15 @@
         <v>483</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>16</v>
       </c>
       <c r="B14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" t="s">
         <v>92</v>
-      </c>
-      <c r="C14" t="s">
-        <v>93</v>
       </c>
       <c r="D14">
         <v>60</v>
@@ -8969,15 +8965,15 @@
         <v>0.7134490740740741</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>16</v>
       </c>
       <c r="B15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" t="s">
         <v>97</v>
-      </c>
-      <c r="C15" t="s">
-        <v>98</v>
       </c>
       <c r="D15">
         <v>42.63</v>
@@ -9016,15 +9012,15 @@
         <v>0.71471064814814811</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
         <v>112</v>
-      </c>
-      <c r="C16" t="s">
-        <v>57</v>
       </c>
       <c r="D16">
         <v>45.44</v>
@@ -9060,15 +9056,15 @@
         <v>0.7159375</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8</v>
       </c>
       <c r="B17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" t="s">
         <v>116</v>
-      </c>
-      <c r="C17" t="s">
-        <v>117</v>
       </c>
       <c r="D17">
         <v>47.42</v>
@@ -9101,15 +9097,15 @@
         <v>0.71835648148148146</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>8</v>
       </c>
       <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
         <v>121</v>
-      </c>
-      <c r="C18" t="s">
-        <v>122</v>
       </c>
       <c r="D18">
         <v>54.9</v>
@@ -9145,15 +9141,15 @@
         <v>0.71986111111111106</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8</v>
       </c>
       <c r="B19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" t="s">
         <v>126</v>
-      </c>
-      <c r="C19" t="s">
-        <v>127</v>
       </c>
       <c r="D19">
         <v>46.2</v>
@@ -9192,15 +9188,15 @@
         <v>0.72103009259259254</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>8</v>
       </c>
       <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
         <v>132</v>
-      </c>
-      <c r="C20" t="s">
-        <v>62</v>
       </c>
       <c r="D20">
         <v>38.33</v>
@@ -9236,15 +9232,15 @@
         <v>0.72212962962962968</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8</v>
       </c>
       <c r="B21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" t="s">
         <v>141</v>
-      </c>
-      <c r="C21" t="s">
-        <v>142</v>
       </c>
       <c r="D21">
         <v>60</v>
@@ -9280,15 +9276,15 @@
         <v>0.72354166666666664</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8</v>
       </c>
       <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
         <v>155</v>
-      </c>
-      <c r="C22" t="s">
-        <v>117</v>
       </c>
       <c r="D22">
         <v>60</v>
@@ -9324,15 +9320,15 @@
         <v>0.72526620370370365</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>12</v>
       </c>
       <c r="B23" t="s">
+        <v>167</v>
+      </c>
+      <c r="C23" t="s">
         <v>166</v>
-      </c>
-      <c r="C23" t="s">
-        <v>167</v>
       </c>
       <c r="D23">
         <v>60</v>
@@ -9368,15 +9364,15 @@
         <v>0.72813657407407406</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>12</v>
       </c>
       <c r="B24" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" t="s">
         <v>171</v>
-      </c>
-      <c r="C24" t="s">
-        <v>172</v>
       </c>
       <c r="D24">
         <v>48.46</v>
@@ -9415,15 +9411,15 @@
         <v>0.72946759259259264</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20</v>
       </c>
       <c r="B25" t="s">
+        <v>237</v>
+      </c>
+      <c r="C25" t="s">
         <v>416</v>
-      </c>
-      <c r="C25" t="s">
-        <v>237</v>
       </c>
       <c r="D25">
         <v>48.56</v>
@@ -9459,15 +9455,15 @@
         <v>0.73171296296296295</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
       <c r="B26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" t="s">
         <v>177</v>
-      </c>
-      <c r="C26" t="s">
-        <v>98</v>
       </c>
       <c r="D26">
         <v>42.57</v>
@@ -9509,15 +9505,15 @@
         <v>0.73311342592592588</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20</v>
       </c>
       <c r="B27" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" t="s">
         <v>190</v>
-      </c>
-      <c r="C27" t="s">
-        <v>191</v>
       </c>
       <c r="D27">
         <v>51.02</v>
@@ -9553,15 +9549,15 @@
         <v>0.73454861111111114</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20</v>
       </c>
       <c r="B28" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28" t="s">
         <v>196</v>
-      </c>
-      <c r="C28" t="s">
-        <v>197</v>
       </c>
       <c r="D28">
         <v>45.24</v>
@@ -9591,15 +9587,15 @@
         <v>0.73619212962962965</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20</v>
       </c>
       <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
         <v>201</v>
-      </c>
-      <c r="C29" t="s">
-        <v>78</v>
       </c>
       <c r="D29">
         <v>53.49</v>
@@ -9632,15 +9628,15 @@
         <v>0.73753472222222227</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>20</v>
       </c>
       <c r="B30" t="s">
+        <v>206</v>
+      </c>
+      <c r="C30" t="s">
         <v>205</v>
-      </c>
-      <c r="C30" t="s">
-        <v>206</v>
       </c>
       <c r="D30">
         <v>49.15</v>
@@ -9673,15 +9669,15 @@
         <v>0.73881944444444447</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20</v>
       </c>
       <c r="B31" t="s">
+        <v>211</v>
+      </c>
+      <c r="C31" t="s">
         <v>210</v>
-      </c>
-      <c r="C31" t="s">
-        <v>211</v>
       </c>
       <c r="D31">
         <v>57.62</v>
@@ -9711,15 +9707,15 @@
         <v>0.74023148148148143</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>20</v>
       </c>
       <c r="B32" t="s">
+        <v>216</v>
+      </c>
+      <c r="C32" t="s">
         <v>215</v>
-      </c>
-      <c r="C32" t="s">
-        <v>216</v>
       </c>
       <c r="D32">
         <v>60</v>
@@ -9749,15 +9745,15 @@
         <v>0.74167824074074074</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>20</v>
       </c>
       <c r="B33" t="s">
+        <v>222</v>
+      </c>
+      <c r="C33" t="s">
         <v>221</v>
-      </c>
-      <c r="C33" t="s">
-        <v>222</v>
       </c>
       <c r="D33">
         <v>39.799999999999997</v>
@@ -9787,15 +9783,15 @@
         <v>0.74274305555555553</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>20</v>
       </c>
       <c r="B34" t="s">
+        <v>227</v>
+      </c>
+      <c r="C34" t="s">
         <v>226</v>
-      </c>
-      <c r="C34" t="s">
-        <v>227</v>
       </c>
       <c r="D34">
         <v>46.6</v>
@@ -9828,15 +9824,15 @@
         <v>0.74405092592592592</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>20</v>
       </c>
       <c r="B35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C35" t="s">
         <v>231</v>
-      </c>
-      <c r="C35" t="s">
-        <v>232</v>
       </c>
       <c r="D35">
         <v>53.8</v>
@@ -9869,15 +9865,15 @@
         <v>0.74534722222222227</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20</v>
       </c>
       <c r="B36" t="s">
+        <v>237</v>
+      </c>
+      <c r="C36" t="s">
         <v>236</v>
-      </c>
-      <c r="C36" t="s">
-        <v>237</v>
       </c>
       <c r="D36">
         <v>53.42</v>

</xml_diff>